<commit_message>
get from excel by column name
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -4,48 +4,121 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="23640" windowHeight="5205"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="AmazonBooks" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
-  <si>
-    <t>TestCaseName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>Apache_POI_TC</t>
-  </si>
-  <si>
-    <t>testuser_1</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>Chrome</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>To Kill a Mockingbid</t>
+  </si>
+  <si>
+    <t>Jane Austin</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Classic</t>
+  </si>
+  <si>
+    <t>Haper Lee</t>
+  </si>
+  <si>
+    <t>Harper Collins</t>
+  </si>
+  <si>
+    <t>George Orwell</t>
+  </si>
+  <si>
+    <t>Persuation</t>
+  </si>
+  <si>
+    <t>Pride and Prejudice</t>
+  </si>
+  <si>
+    <t>Tail of Two Cities</t>
+  </si>
+  <si>
+    <t>Charles Dickens</t>
+  </si>
+  <si>
+    <t>Oliver Twist</t>
+  </si>
+  <si>
+    <t>Winds of Winter</t>
+  </si>
+  <si>
+    <t>George R. R. Martin</t>
+  </si>
+  <si>
+    <t>A Dance of Dragons</t>
+  </si>
+  <si>
+    <t>Honor Harrington</t>
+  </si>
+  <si>
+    <t>David Weber</t>
+  </si>
+  <si>
+    <t>Gust Front</t>
+  </si>
+  <si>
+    <t>John Ringo</t>
+  </si>
+  <si>
+    <t>Baen</t>
+  </si>
+  <si>
+    <t>Simon and Schuster</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>Science Fiction</t>
+  </si>
+  <si>
+    <t>Drama</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>12/23/1815</t>
+  </si>
+  <si>
+    <t>12/1/1817</t>
+  </si>
+  <si>
+    <t>1/28/1813</t>
+  </si>
+  <si>
+    <t>1/14/1859</t>
+  </si>
+  <si>
+    <t>File Read and comment written</t>
   </si>
 </sst>
 </file>
@@ -53,28 +126,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,24 +152,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -400,81 +480,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="6" customWidth="true" width="27.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>22108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>1984</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>18057</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>1838</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
+        <v>40555</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>2001</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>